<commit_message>
feature/be: ORM 적용 및 인증 추가
</commit_message>
<xml_diff>
--- a/apps/conveyor/backend/sbin/R301.xlsx
+++ b/apps/conveyor/backend/sbin/R301.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/works/semi-ts/conveyor/monorepo/apps/conveyor/backend/sbin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FCEB61-4F07-BB49-86FE-B7B253529076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DEE4B7-8B4F-6C43-93C7-AA0F477C4C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="51200" windowHeight="24880" tabRatio="812" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1020" windowWidth="51200" windowHeight="24880" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="282">
   <si>
     <t>Domain</t>
   </si>
@@ -343,9 +343,6 @@
   </si>
   <si>
     <t>alarminfo</t>
-  </si>
-  <si>
-    <t>alarminfo</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1043,6 +1040,62 @@
   </si>
   <si>
     <t>UQ_TIMESTAMP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alarminfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompleteCarrier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompletecarrierCount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DestinationCount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DestinationZone</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OperationLogs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskTransferInfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskTransferInfoStatus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WarningInfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZoneDynamicAttributes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZoneInfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZoneOccupiedAttributes</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1179,7 +1232,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1235,7 +1288,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1521,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22:P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -1574,17 +1636,17 @@
         <v>53</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1602,7 +1664,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1610,17 +1672,17 @@
         <v>53</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1628,17 +1690,17 @@
         <v>53</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>79</v>
+        <v>270</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1646,17 +1708,17 @@
         <v>53</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>80</v>
+        <v>271</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1664,17 +1726,17 @@
         <v>53</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>87</v>
+        <v>272</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1682,17 +1744,17 @@
         <v>53</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>91</v>
+        <v>273</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1700,17 +1762,17 @@
         <v>53</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1718,21 +1780,21 @@
         <v>53</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1740,21 +1802,21 @@
         <v>53</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1762,17 +1824,17 @@
         <v>53</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>131</v>
+        <v>275</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1780,17 +1842,17 @@
         <v>53</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>132</v>
+        <v>276</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1798,17 +1860,17 @@
         <v>53</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>139</v>
+        <v>277</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1816,17 +1878,17 @@
         <v>53</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1834,164 +1896,169 @@
         <v>53</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>144</v>
+        <v>278</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>150</v>
+        <v>279</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>153</v>
+        <v>280</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>156</v>
+        <v>281</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="B20" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="E20" s="17"/>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="9" t="s">
+      <c r="C21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="I22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="J22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="K22" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="9" t="s">
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="I23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="J23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="K23" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="9" t="s">
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="I24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="J24" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="I25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="K25" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="9" t="s">
-        <v>165</v>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2049,7 +2116,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>28</v>
@@ -2071,7 +2138,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>22</v>
@@ -2084,12 +2151,12 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>22</v>
@@ -2102,15 +2169,15 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2118,7 +2185,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="14"/>
       <c r="H5" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2132,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2168,7 +2235,7 @@
         <v>40</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>12</v>
@@ -2176,10 +2243,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -2198,10 +2265,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -2211,19 +2278,19 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -2233,19 +2300,19 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
@@ -2255,15 +2322,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2271,7 +2338,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2330,10 +2397,10 @@
     </row>
     <row r="2" spans="1:8" ht="17">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -2350,7 +2417,7 @@
     </row>
     <row r="3" spans="1:8" ht="17">
       <c r="A3" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
@@ -2363,19 +2430,19 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17">
       <c r="A4" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -2384,18 +2451,18 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17">
       <c r="A5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
@@ -2405,15 +2472,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17">
       <c r="A6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2421,15 +2488,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17">
       <c r="A7" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -2437,15 +2504,15 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17">
       <c r="A8" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -2453,15 +2520,15 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17">
       <c r="A9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -2469,15 +2536,15 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17">
       <c r="A10" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -2485,15 +2552,15 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17">
       <c r="A11" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -2501,15 +2568,15 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17">
       <c r="A12" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -2517,15 +2584,15 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17">
       <c r="A13" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2533,15 +2600,15 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17">
       <c r="A14" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2549,15 +2616,15 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17">
       <c r="A15" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2565,7 +2632,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2623,10 +2690,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -2643,10 +2710,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -2656,17 +2723,17 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -2679,17 +2746,17 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="6"/>
     </row>
@@ -2748,10 +2815,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -2768,10 +2835,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -2786,10 +2853,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -2798,7 +2865,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H4" s="6"/>
     </row>
@@ -2854,10 +2921,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -2874,7 +2941,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
@@ -2889,15 +2956,15 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -2905,15 +2972,15 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2921,15 +2988,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2937,15 +3004,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -2953,12 +3020,12 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>48</v>
@@ -2969,7 +3036,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3026,10 +3093,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -3041,17 +3108,17 @@
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -3061,12 +3128,12 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>48</v>
@@ -3079,25 +3146,25 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3154,10 +3221,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -3174,10 +3241,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -3187,19 +3254,19 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -3207,15 +3274,15 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -3223,15 +3290,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -3239,15 +3306,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -3255,33 +3322,33 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -3289,7 +3356,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3348,10 +3415,10 @@
     </row>
     <row r="2" spans="1:8" ht="12" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -3368,10 +3435,10 @@
     </row>
     <row r="3" spans="1:8" ht="17">
       <c r="A3" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -3389,7 +3456,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -3399,15 +3466,15 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17">
       <c r="A5" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
@@ -3417,15 +3484,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17">
       <c r="A6" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>16</v>
@@ -3434,10 +3501,10 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3491,10 +3558,10 @@
     </row>
     <row r="2" spans="1:7" ht="17">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -3510,10 +3577,10 @@
     </row>
     <row r="3" spans="1:7" ht="17">
       <c r="A3" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -3523,18 +3590,18 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17">
       <c r="A4" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -3543,7 +3610,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3558,7 +3625,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1"/>
@@ -3601,7 +3668,7 @@
     </row>
     <row r="2" spans="1:8" ht="17">
       <c r="A2" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>28</v>
@@ -3613,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6">
-        <v>1</v>
+        <v>100001</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3623,10 +3690,10 @@
     </row>
     <row r="3" spans="1:8" ht="17">
       <c r="A3" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>249</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>14</v>
@@ -3636,19 +3703,19 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17">
       <c r="A4" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>14</v>
@@ -3658,15 +3725,15 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17">
       <c r="A5" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>14</v>
@@ -3676,50 +3743,50 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A6" s="19" t="s">
+      <c r="B6" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A7" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A8" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="6"/>
@@ -3727,24 +3794,24 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A9" s="19" t="s">
-        <v>264</v>
-      </c>
       <c r="B9" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="19" t="s">
-        <v>265</v>
+      <c r="H9" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3802,10 +3869,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -3824,10 +3891,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -3837,19 +3904,19 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -3859,15 +3926,15 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -3875,15 +3942,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -3891,15 +3958,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -3907,15 +3974,15 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -3923,15 +3990,15 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -3939,25 +4006,25 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4015,10 +4082,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -4035,7 +4102,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
@@ -4050,15 +4117,15 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -4068,7 +4135,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4076,7 +4143,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -4084,15 +4151,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -4100,15 +4167,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -4116,7 +4183,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4173,10 +4240,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -4193,10 +4260,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -4206,19 +4273,19 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -4228,15 +4295,15 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
@@ -4246,7 +4313,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -4304,10 +4371,10 @@
     </row>
     <row r="2" spans="1:8" ht="17">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -4324,7 +4391,7 @@
     </row>
     <row r="3" spans="1:8" ht="17">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
@@ -4339,15 +4406,15 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17">
       <c r="A4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -4360,10 +4427,10 @@
     </row>
     <row r="5" spans="1:8" ht="17">
       <c r="A5" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
@@ -4373,15 +4440,15 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17">
       <c r="A6" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -4389,15 +4456,15 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17">
       <c r="A7" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -4405,15 +4472,15 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17">
       <c r="A8" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -4421,15 +4488,15 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17">
       <c r="A9" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -4437,15 +4504,15 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17">
       <c r="A10" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -4453,15 +4520,15 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17">
       <c r="A11" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -4469,7 +4536,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -4841,7 +4908,7 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17">
@@ -4859,7 +4926,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4953,7 +5020,7 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4971,7 +5038,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4989,7 +5056,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5009,7 +5076,7 @@
         <v>75</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5025,7 +5092,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5041,7 +5108,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5059,7 +5126,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5075,7 +5142,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5093,7 +5160,7 @@
         <v>61</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5109,7 +5176,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -5200,7 +5267,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -5293,7 +5360,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>28</v>
@@ -5327,7 +5394,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" s="6"/>
     </row>
@@ -5420,13 +5487,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="6" t="b">
         <v>1</v>
@@ -5442,36 +5509,36 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="14"/>
@@ -5479,21 +5546,21 @@
         <v>61</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -5501,7 +5568,7 @@
         <v>62</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature/fe : DBM 작업 진행 중,,
</commit_message>
<xml_diff>
--- a/apps/conveyor/backend/sbin/R301.xlsx
+++ b/apps/conveyor/backend/sbin/R301.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/works/semi-ts/conveyor/monorepo/apps/conveyor/backend/sbin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DEE4B7-8B4F-6C43-93C7-AA0F477C4C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C364A7-3A63-554A-AD6B-FC2F97E984A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="51200" windowHeight="24880" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1020" windowWidth="51200" windowHeight="24880" tabRatio="812" firstSheet="3" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="zonedynamicattributes" sheetId="14" r:id="rId21"/>
     <sheet name="zoneInfo" sheetId="57" r:id="rId22"/>
     <sheet name="zoneoccupiedattributes" sheetId="17" r:id="rId23"/>
+    <sheet name="MsgQueue" sheetId="74" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="296">
   <si>
     <t>Domain</t>
   </si>
@@ -1096,6 +1097,62 @@
   </si>
   <si>
     <t>ZoneOccupiedAttributes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MsgQueue</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>임시 메모리 테이블</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>State</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(20000)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Channel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(256)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:Wait, 2: Work, 9: Fail</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(1024)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>에러 메시지 기록</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1232,7 +1289,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1288,16 +1345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1583,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22:P25"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -1598,14 +1646,15 @@
     <col min="5" max="5" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1640625" style="8" customWidth="1"/>
-    <col min="10" max="11" width="4.6640625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="8"/>
+    <col min="8" max="8" width="11.33203125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="68.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" style="8" customWidth="1"/>
+    <col min="11" max="12" width="4.6640625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1628,10 +1677,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
         <v>53</v>
       </c>
@@ -1645,11 +1697,12 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="9" t="s">
         <v>53</v>
       </c>
@@ -1663,29 +1716,31 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="19" t="s">
         <v>76</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
         <v>53</v>
       </c>
@@ -1699,11 +1754,12 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="9" t="s">
         <v>53</v>
       </c>
@@ -1717,11 +1773,12 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="9" t="s">
         <v>53</v>
       </c>
@@ -1735,11 +1792,12 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="9" t="s">
         <v>53</v>
       </c>
@@ -1753,11 +1811,12 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="9" t="s">
         <v>53</v>
       </c>
@@ -1771,11 +1830,12 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="9" t="s">
         <v>53</v>
       </c>
@@ -1793,18 +1853,19 @@
         <v>115</v>
       </c>
       <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="19" t="s">
         <v>122</v>
       </c>
       <c r="D11" s="11"/>
@@ -1815,11 +1876,12 @@
         <v>85</v>
       </c>
       <c r="G11" s="11"/>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="9" t="s">
         <v>53</v>
       </c>
@@ -1833,47 +1895,50 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="11"/>
+      <c r="I12" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="19" t="s">
         <v>131</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="11"/>
+      <c r="I13" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="19" t="s">
         <v>138</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="9" t="s">
         <v>53</v>
       </c>
@@ -1887,11 +1952,12 @@
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="11"/>
+      <c r="I15" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
         <v>53</v>
       </c>
@@ -1905,11 +1971,12 @@
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="11"/>
+      <c r="I16" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="A17" s="9" t="s">
         <v>53</v>
       </c>
@@ -1927,11 +1994,12 @@
         <v>85</v>
       </c>
       <c r="G17" s="11"/>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="11"/>
+      <c r="I17" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="A18" s="9" t="s">
         <v>53</v>
       </c>
@@ -1945,11 +2013,12 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="A19" s="9" t="s">
         <v>53</v>
       </c>
@@ -1967,21 +2036,33 @@
         <v>85</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:16">
+    <row r="20" spans="1:17">
+      <c r="A20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="18" t="s">
         <v>33</v>
       </c>
@@ -1989,80 +2070,86 @@
       <c r="E21" s="17"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:16">
-      <c r="I22" s="9" t="s">
+    <row r="22" spans="1:17">
+      <c r="J22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="K22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="L22" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="9" t="s">
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="I23" s="9" t="s">
+    <row r="23" spans="1:17">
+      <c r="J23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="K23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="L23" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
-      <c r="I24" s="9" t="s">
+    <row r="24" spans="1:17">
+      <c r="J24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="K24" s="10" t="s">
+      <c r="L24" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L24" s="11"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="9" t="s">
+      <c r="P24" s="11"/>
+      <c r="Q24" s="9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="I25" s="9" t="s">
+    <row r="25" spans="1:17">
+      <c r="J25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="K25" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="K25" s="10" t="s">
+      <c r="L25" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="L25" s="11"/>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
-      <c r="P25" s="9" t="s">
+      <c r="P25" s="11"/>
+      <c r="Q25" s="9" t="s">
         <v>164</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" location="alarminfo!A1" display="alarminfo" xr:uid="{728D3F7B-6B78-524D-AA14-34ECF6C7ADB1}"/>
+    <hyperlink ref="C11" location="logs!A1" display="logs" xr:uid="{E36C9800-5765-1448-8E86-1BF59E46E6B4}"/>
+    <hyperlink ref="C13" location="tasktransferinfo!A1" display="tasktransferinfo" xr:uid="{72E07564-6F0E-CB4A-9D33-38D596C2C88D}"/>
+    <hyperlink ref="C14" location="tasktransferinfostatus!A1" display="tasktransferinfostatus" xr:uid="{6257E857-8359-C847-8593-20006ED8AE5A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2880,7 +2967,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -3179,7 +3266,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -4327,8 +4414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -4550,6 +4637,238 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C2246E-4600-3D41-A196-B22221A44C48}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17">
+      <c r="A2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="17">
+      <c r="A3" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="17">
+      <c r="A4" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17">
+      <c r="A5" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="17">
+      <c r="A6" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="17">
+      <c r="A7" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="17">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="17">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="17">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="17">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="17">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="17">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="H22" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4940,9 +5259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D1965B-20A4-4313-9322-BFE9A22AFA8E}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>

</xml_diff>

<commit_message>
feature/be: DBM 로그 저장 기능 추가
</commit_message>
<xml_diff>
--- a/apps/conveyor/backend/sbin/R301.xlsx
+++ b/apps/conveyor/backend/sbin/R301.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/works/semi-ts/conveyor/monorepo/apps/conveyor/backend/sbin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C364A7-3A63-554A-AD6B-FC2F97E984A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79611A61-A8A9-6A44-96CF-394BCE93D0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="51200" windowHeight="24880" tabRatio="812" firstSheet="3" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1020" windowWidth="32360" windowHeight="25340" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="301">
   <si>
     <t>Domain</t>
   </si>
@@ -1153,6 +1153,26 @@
   </si>
   <si>
     <t>에러 메시지 기록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_START_TIME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX_END_TIME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Log EventID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(16)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventCode</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1633,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -1747,7 +1767,7 @@
       <c r="B5" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D5" s="9"/>
@@ -1766,7 +1786,7 @@
       <c r="B6" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="19" t="s">
         <v>79</v>
       </c>
       <c r="D6" s="9"/>
@@ -1964,7 +1984,7 @@
       <c r="B16" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="19" t="s">
         <v>143</v>
       </c>
       <c r="D16" s="11"/>
@@ -1983,7 +2003,7 @@
       <c r="B17" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="19" t="s">
         <v>149</v>
       </c>
       <c r="D17" s="11"/>
@@ -2149,6 +2169,10 @@
     <hyperlink ref="C11" location="logs!A1" display="logs" xr:uid="{E36C9800-5765-1448-8E86-1BF59E46E6B4}"/>
     <hyperlink ref="C13" location="tasktransferinfo!A1" display="tasktransferinfo" xr:uid="{72E07564-6F0E-CB4A-9D33-38D596C2C88D}"/>
     <hyperlink ref="C14" location="tasktransferinfostatus!A1" display="tasktransferinfostatus" xr:uid="{6257E857-8359-C847-8593-20006ED8AE5A}"/>
+    <hyperlink ref="C5" location="completecarrier!A1" display="completecarrier" xr:uid="{178E308D-0C97-954F-9BC0-576AD2FA8966}"/>
+    <hyperlink ref="C6" location="abortedcarriercount!A1" display="completecarriercount" xr:uid="{E5D70720-6D93-824A-8FAE-3F3894189C3F}"/>
+    <hyperlink ref="C16" location="warninginfo!A1" display="warninginfo" xr:uid="{18C038CC-FE53-B34D-B1F6-0A5360725784}"/>
+    <hyperlink ref="C17" location="zonedynamicattributes!A1" display="zonedynamicattributes" xr:uid="{9ED9EB82-D7FE-9944-A88C-02E45371993B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2964,10 +2988,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -3048,10 +3072,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>123</v>
+        <v>300</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>92</v>
+        <v>299</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -3059,12 +3083,12 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>200</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>92</v>
@@ -3075,12 +3099,12 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>92</v>
@@ -3091,12 +3115,12 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>92</v>
@@ -3107,15 +3131,15 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" customHeight="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="6" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -3123,6 +3147,22 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3266,7 +3306,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -3424,7 +3464,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>100</v>
+        <v>296</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>213</v>
@@ -3441,7 +3481,9 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>297</v>
+      </c>
       <c r="H9" s="6" t="s">
         <v>214</v>
       </c>
@@ -3912,9 +3954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
@@ -4644,7 +4684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C2246E-4600-3D41-A196-B22221A44C48}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -5507,8 +5547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B75199B-2B5B-45F9-B8D5-0B3A59208DF0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1"/>

</xml_diff>

<commit_message>
feature/be : zone 초기화 작업
</commit_message>
<xml_diff>
--- a/apps/conveyor/backend/sbin/R301.xlsx
+++ b/apps/conveyor/backend/sbin/R301.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/works/semi-ts/conveyor/monorepo/apps/conveyor/backend/sbin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79611A61-A8A9-6A44-96CF-394BCE93D0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431BEABE-F089-714B-AE07-4E5B54132797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1020" windowWidth="32360" windowHeight="25340" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,7 @@
     <sheet name="zoneInfo" sheetId="57" r:id="rId22"/>
     <sheet name="zoneoccupiedattributes" sheetId="17" r:id="rId23"/>
     <sheet name="MsgQueue" sheetId="74" r:id="rId24"/>
+    <sheet name="zoneStats" sheetId="75" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="313">
   <si>
     <t>Domain</t>
   </si>
@@ -1173,6 +1174,54 @@
   </si>
   <si>
     <t>EventCode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZoneStats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zone 통계 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UQ_ZONE_STAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoneId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seq_no</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>집계 일자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrierNum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarmNum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>warningNum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoneStats</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1309,7 +1358,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1366,6 +1415,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1651,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -2068,7 +2120,7 @@
       <c r="B20" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="19" t="s">
         <v>283</v>
       </c>
       <c r="D20" s="9"/>
@@ -2083,40 +2135,41 @@
       </c>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="20" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="J22" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9" t="s">
-        <v>164</v>
-      </c>
+      <c r="C22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22"/>
     </row>
     <row r="23" spans="1:17">
       <c r="J23" s="9" t="s">
         <v>53</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -2130,18 +2183,18 @@
       <c r="J24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="11" t="s">
-        <v>120</v>
+      <c r="K24" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
+        <v>57</v>
+      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
       <c r="Q24" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2149,16 +2202,34 @@
         <v>53</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="J26" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="9" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2173,6 +2244,7 @@
     <hyperlink ref="C6" location="abortedcarriercount!A1" display="completecarriercount" xr:uid="{E5D70720-6D93-824A-8FAE-3F3894189C3F}"/>
     <hyperlink ref="C16" location="warninginfo!A1" display="warninginfo" xr:uid="{18C038CC-FE53-B34D-B1F6-0A5360725784}"/>
     <hyperlink ref="C17" location="zonedynamicattributes!A1" display="zonedynamicattributes" xr:uid="{9ED9EB82-D7FE-9944-A88C-02E45371993B}"/>
+    <hyperlink ref="C20" location="MsgQueue!A1" display="MsgQueue" xr:uid="{7041FF3B-10DC-E44C-AA48-B18E619C327B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4685,7 +4757,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -4827,6 +4899,248 @@
       <c r="H7" s="6" t="s">
         <v>295</v>
       </c>
+    </row>
+    <row r="8" spans="1:8" ht="17">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="17">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="17">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="17">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="17">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="17">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="17">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="H22" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8610810-D77B-4E45-9D28-E1D6D993E934}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17">
+      <c r="A2" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="17">
+      <c r="A3" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17">
+      <c r="A4" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17">
+      <c r="A5" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="17">
+      <c r="A6" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="17">
+      <c r="A7" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="17">
       <c r="A8" s="6"/>

</xml_diff>